<commit_message>
Changed structure (to make easy to run)
</commit_message>
<xml_diff>
--- a/Statistics/TestCases/Spl_2.xlsx
+++ b/Statistics/TestCases/Spl_2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nepathak/Internship_Neetish/socketcomm/Statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nepathak/Internship_Neetish/socketcomm/Statistics/TestCases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="3060" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="5080" yWindow="2860" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Latency_C" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>AEAD_ECDSA256_X25519</t>
+  </si>
+  <si>
+    <t>ECDHE_ECDSA256_X25519</t>
   </si>
 </sst>
 </file>
@@ -15413,15 +15416,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1001"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>